<commit_message>
Some fixes, notably in tests
</commit_message>
<xml_diff>
--- a/tests/data/assembly_report/example_echo_plate.xlsx
+++ b/tests/data/assembly_report/example_echo_plate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="content" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="volume" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="concentration" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="volume (ul)" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="concentration (ng-ul)" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -476,8 +476,8 @@
   </sheetPr>
   <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y17" activeCellId="0" sqref="Y17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y16" activeCellId="0" sqref="Y16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1308,8 +1308,8 @@
   </sheetPr>
   <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y16" activeCellId="0" sqref="Y16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y17" activeCellId="0" sqref="Y17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1396,22 +1396,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="G2" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="H2" s="3" t="n">
         <v>0</v>
@@ -1473,22 +1473,22 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="G3" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="H3" s="3" t="n">
         <v>0</v>
@@ -1550,22 +1550,22 @@
         <v>14</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="H4" s="3" t="n">
         <v>0</v>
@@ -1627,22 +1627,22 @@
         <v>21</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="G5" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="H5" s="3" t="n">
         <v>0</v>
@@ -1704,22 +1704,22 @@
         <v>28</v>
       </c>
       <c r="B6" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="G6" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="H6" s="3" t="n">
         <v>0</v>
@@ -1781,22 +1781,22 @@
         <v>35</v>
       </c>
       <c r="B7" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="G7" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="H7" s="3" t="n">
         <v>0</v>
@@ -1858,22 +1858,22 @@
         <v>42</v>
       </c>
       <c r="B8" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="G8" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="H8" s="3" t="n">
         <v>0</v>
@@ -1935,22 +1935,22 @@
         <v>49</v>
       </c>
       <c r="B9" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="D9" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="F9" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="G9" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="H9" s="3" t="n">
         <v>0</v>
@@ -2012,22 +2012,22 @@
         <v>56</v>
       </c>
       <c r="B10" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="F10" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="G10" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="H10" s="3" t="n">
         <v>0</v>
@@ -2089,22 +2089,22 @@
         <v>63</v>
       </c>
       <c r="B11" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="G11" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="H11" s="3" t="n">
         <v>0</v>
@@ -2166,22 +2166,22 @@
         <v>70</v>
       </c>
       <c r="B12" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="C12" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="D12" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="G12" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="H12" s="3" t="n">
         <v>0</v>
@@ -2243,22 +2243,22 @@
         <v>77</v>
       </c>
       <c r="B13" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="C13" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="D13" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="F13" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="G13" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="H13" s="3" t="n">
         <v>0</v>
@@ -2320,19 +2320,19 @@
         <v>84</v>
       </c>
       <c r="B14" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="C14" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="D14" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="G14" s="3" t="n">
         <v>0</v>
@@ -2397,19 +2397,19 @@
         <v>90</v>
       </c>
       <c r="B15" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="C15" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="D15" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="G15" s="3" t="n">
         <v>0</v>
@@ -2474,19 +2474,19 @@
         <v>96</v>
       </c>
       <c r="B16" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="C16" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="D16" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="G16" s="3" t="n">
         <v>0</v>
@@ -2543,7 +2543,7 @@
         <v>0</v>
       </c>
       <c r="Y16" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2551,19 +2551,19 @@
         <v>103</v>
       </c>
       <c r="B17" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="C17" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="D17" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="F17" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
       <c r="G17" s="3" t="n">
         <v>0</v>
@@ -2620,10 +2620,12 @@
         <v>0</v>
       </c>
       <c r="Y17" s="3" t="n">
-        <v>5E-005</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.3" right="0.3" top="0.609722222222222" bottom="0.370138888888889" header="0.1" footer="0.1"/>
@@ -2642,8 +2644,8 @@
   </sheetPr>
   <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X21" activeCellId="0" sqref="X21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y16" activeCellId="0" sqref="Y16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>